<commit_message>
Updated an excel sheet
</commit_message>
<xml_diff>
--- a/documents/movies.xlsx
+++ b/documents/movies.xlsx
@@ -1,108 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20711"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1059C7C4-3D62-4AC3-938F-AEA49342C69C}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020"/>
+  <definedNames/>
+  <calcPr calcId="179020" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Admissions
-(millions)</t>
-  </si>
-  <si>
-    <t>Title (year) (studio)</t>
-  </si>
-  <si>
-    <t>Director(s)</t>
-  </si>
-  <si>
-    <t>Gone With the Wind (1939) (MGM)</t>
-  </si>
-  <si>
-    <t>Victor Fleming, George Cukor, Sam Wood</t>
-  </si>
-  <si>
-    <t>Star Wars (Ep. IV: A New Hope) (1977) (Fox)</t>
-  </si>
-  <si>
-    <t>George Lucas</t>
-  </si>
-  <si>
-    <t>ET: The Extra-Terrestrial (1982) (Univ)</t>
-  </si>
-  <si>
-    <t>Steven Spielberg</t>
-  </si>
-  <si>
-    <t>The Sound of Music (1965) (Fox)</t>
-  </si>
-  <si>
-    <t>Robert Wise</t>
-  </si>
-  <si>
-    <t>The Ten Commandments (1956) (Para)</t>
-  </si>
-  <si>
-    <t>Cecil B. DeMille</t>
-  </si>
-  <si>
-    <t>Titanic (1997) (Fox)</t>
-  </si>
-  <si>
-    <t>James Cameron</t>
-  </si>
-  <si>
-    <t>Snow White and the Seven Dwarfs (1937) (BV)</t>
-  </si>
-  <si>
-    <t>David Hand</t>
-  </si>
-  <si>
-    <t>Jaws (1975) (Univ)</t>
-  </si>
-  <si>
-    <t>Doctor Zhivago (1965) (MGM)</t>
-  </si>
-  <si>
-    <t>David Lean</t>
-  </si>
-  <si>
-    <t>The Lion King (1994) (BV)</t>
-  </si>
-  <si>
-    <t>Roger Allers, Rob Minkoff</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -121,25 +46,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0">
+      <text>
+        <t>CHanged text automatically</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,172 +437,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col width="11.7109375" customWidth="1" min="2" max="2"/>
+    <col width="39.7109375" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="27.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Admissions
+(millions)</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Title (year) (studio)</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Director(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="n">
+        <v>225.7</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gone With the Wind (1939) (MGM)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Victor Fleming, George Cukor, Sam Wood</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="n">
+        <v>194.4</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Star Wars (Ep. IV: A New Hope) (1977) (Fox)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>George Lucas</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>225.7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="n">
+        <v>161</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ET: The Extra-Terrestrial (1982) (Univ)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Spielberg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B5" t="n">
+        <v>156.4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>The Sound of Music (1965) (Fox)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Robert Wise</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>194.4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B6" t="n">
+        <v>130</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The Ten Commandments (1956) (Para)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Cecil B. DeMille</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B7" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Titanic (1997) (Fox)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>James Cameron</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>161</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B8" t="n">
+        <v>126.3</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Snow White and the Seven Dwarfs (1937) (BV)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>David Hand</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B9" t="n">
+        <v>120.7</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Jaws (1975) (Univ)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Steven Spielberg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>156.4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B10" t="n">
+        <v>120.1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Doctor Zhivago (1965) (MGM)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>David Lean</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>130</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>128.4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>126.3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>120.7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>120.1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>118.9</v>
       </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The Lion King (1994) (BV)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Roger Allers, Rob Minkoff</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12">
+        <f>SUM(B2:B11)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>